<commit_message>
added more data to excel file
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/products/pharma_pos.pack.xlsx
+++ b/addons/pharma-pos/demo_excel/products/pharma_pos.pack.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Product</t>
   </si>
@@ -47,6 +47,27 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>Cisflem (Carbo) 125 mg/60 ml Syrup</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>(Amoxicillin) 125 mg/60 ml Syrup</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Mucosolve (Ambroxol) 30 mg/60 ml Syrup</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -390,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -469,6 +490,62 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>100</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>50</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>50</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>